<commit_message>
interactive dashboard with plotly
</commit_message>
<xml_diff>
--- a/pogoda.xlsx
+++ b/pogoda.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2119,6 +2119,272 @@
         </is>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="B45" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D45" t="n">
+        <v>93</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>7.416</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>19:41:35 02-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="B46" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D46" t="n">
+        <v>93</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>7.416</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>19:43:11 02-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="B47" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D47" t="n">
+        <v>93</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>7.416</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>19:45:04 02-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="B48" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D48" t="n">
+        <v>93</v>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>7.416</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>19:52:27 02-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="B49" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D49" t="n">
+        <v>93</v>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>7.416</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>19:55:09 02-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="B50" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D50" t="n">
+        <v>93</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>7.416</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>19:56:52 02-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>-3.06</v>
+      </c>
+      <c r="B51" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1015</v>
+      </c>
+      <c r="D51" t="n">
+        <v>93</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>7.416</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>19:57:34 02-12-2025</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
connection with db - read / write
</commit_message>
<xml_diff>
--- a/pogoda.xlsx
+++ b/pogoda.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2385,6 +2385,158 @@
         </is>
       </c>
     </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>-4.06</v>
+      </c>
+      <c r="B52" t="n">
+        <v>-7.91</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1029</v>
+      </c>
+      <c r="D52" t="n">
+        <v>50</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>9.251999999999999</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>18:38:12 08-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>-4.06</v>
+      </c>
+      <c r="B53" t="n">
+        <v>-7.91</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1029</v>
+      </c>
+      <c r="D53" t="n">
+        <v>50</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>9.251999999999999</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>18:38:29 08-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>-4.06</v>
+      </c>
+      <c r="B54" t="n">
+        <v>-7.91</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1029</v>
+      </c>
+      <c r="D54" t="n">
+        <v>50</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>9.251999999999999</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>18:39:31 08-12-2025</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>-4.06</v>
+      </c>
+      <c r="B55" t="n">
+        <v>-7.91</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1029</v>
+      </c>
+      <c r="D55" t="n">
+        <v>50</v>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>clear sky</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Cracow</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>9.251999999999999</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>18:39:47 08-12-2025</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>